<commit_message>
finish collecting the data of Apache commons codec and fix the Apache commons lang
</commit_message>
<xml_diff>
--- a/data/Apache commons Lang/BMI/Metric 6.xlsx
+++ b/data/Apache commons Lang/BMI/Metric 6.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A75F719-F1B5-4D54-90C6-1F50BACF4883}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B09D160-F780-43FB-A1FF-D8DB2DD98769}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1212" yWindow="924" windowWidth="12624" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6804" yWindow="1524" windowWidth="12612" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -406,10 +406,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>

</xml_diff>